<commit_message>
continuación con la solución del taller.
</commit_message>
<xml_diff>
--- a/taller1Norma.xlsx
+++ b/taller1Norma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\AdminDatabase\AviancaADB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC05EFD-586C-4A23-8276-4055E982D595}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CBBC0E-F1BB-470A-B992-341AAFE97A81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,8 +388,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +415,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -421,14 +434,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,16 +760,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="L5" zoomScale="115" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
@@ -767,29 +782,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -806,7 +821,7 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="M2" t="s">
@@ -890,11 +905,11 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="5" t="s">
         <v>62</v>
       </c>
       <c r="G8" t="s">
@@ -911,7 +926,7 @@
       <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -952,7 +967,7 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G13" t="s">
@@ -974,7 +989,7 @@
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="3"/>
       <c r="E15" t="s">
         <v>3</v>
       </c>
@@ -997,7 +1012,7 @@
       <c r="C17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1012,7 +1027,7 @@
       <c r="I18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="5" t="s">
         <v>71</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -1095,7 +1110,7 @@
       <c r="C22" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="3"/>
       <c r="F22" t="s">
         <v>44</v>
       </c>
@@ -1157,7 +1172,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F27" t="s">
@@ -1187,7 +1202,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>103</v>
       </c>
       <c r="H30" t="s">
@@ -1214,7 +1229,7 @@
       <c r="H33" t="s">
         <v>88</v>
       </c>
-      <c r="K33" s="3"/>
+      <c r="K33" s="2"/>
     </row>
     <row r="34" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H34" t="s">

</xml_diff>

<commit_message>
se ajusta modelo con la tabla logs
</commit_message>
<xml_diff>
--- a/taller1Norma.xlsx
+++ b/taller1Norma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\AdminDatabase\AviancaADB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5FC62-C7C7-4BA2-B351-1E2D524A81A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F080053A-DF70-4BA0-AB66-10356EDC00D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,18 +402,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -440,16 +434,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,16 +759,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="115" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="115" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
@@ -789,29 +782,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="2"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -828,7 +821,7 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="M2" t="s">
@@ -912,11 +905,11 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G8" t="s">
@@ -933,7 +926,7 @@
       <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -974,7 +967,7 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G13" t="s">
@@ -993,10 +986,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
       <c r="E15" t="s">
         <v>3</v>
       </c>
@@ -1016,10 +1009,10 @@
       <c r="A17" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1028,19 +1021,19 @@
       <c r="C18" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="O18" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1123,7 +1116,7 @@
       <c r="C22" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="2"/>
       <c r="F22" t="s">
         <v>44</v>
       </c>
@@ -1187,10 +1180,10 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1198,7 +1191,7 @@
       <c r="A30" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>100</v>
       </c>
       <c r="H30" t="s">
@@ -1234,7 +1227,7 @@
       <c r="H33" t="s">
         <v>86</v>
       </c>
-      <c r="K33" s="2"/>
+      <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1250,7 +1243,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>96</v>
       </c>
       <c r="H36" t="s">

</xml_diff>